<commit_message>
add some changes like (Method clean and redevelop)
</commit_message>
<xml_diff>
--- a/RESTAssuredAutomation/src/test/resources/SearchPayload.xlsx
+++ b/RESTAssuredAutomation/src/test/resources/SearchPayload.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>category</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>pType</t>
+  </si>
+  <si>
+    <t>showCnt</t>
   </si>
   <si>
     <t>S</t>
@@ -1180,15 +1183,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="3"/>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:8">
+    <row r="1" customHeight="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1213,13 +1216,16 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" customHeight="1" spans="1:8">
+    <row r="2" customHeight="1" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
         <v>500000</v>
@@ -1234,15 +1240,18 @@
         <v>6403</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:9">
+      <c r="A3" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:8">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>10002</v>
@@ -1260,10 +1269,42 @@
         <v>6146</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" s="2">
         <v>10002</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:9">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>500000</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5000000</v>
+      </c>
+      <c r="E4" s="2">
+        <v>11701</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6403</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>